<commit_message>
同步 vivo xiaomi cjj 礼包配置
</commit_message>
<xml_diff>
--- a/config_11.17/shoping_config.xlsx
+++ b/config_11.17/shoping_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28125" windowHeight="12540" tabRatio="533" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28125" windowHeight="12540" tabRatio="533" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tge|标签配置" sheetId="6" r:id="rId1"/>
@@ -7608,13 +7608,16 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>{type="permission_class",class_value = "hlqjd_029_v1v3" }</t>
-  </si>
-  <si>
-    <t>{type="permission_class",class_value = "hlqjd_029_v4v7" }</t>
-  </si>
-  <si>
-    <t>{type="permission_class",class_value = "hlqjd_029_v8v10" }</t>
+    <t>{type="permission_class",class_value = "hlqjd_029_hlqjd_v1" }</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>{type="permission_class",class_value = "hlqjd_029_hlqjd_v4" }</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>{type="permission_class",class_value = "hlqjd_029_hlqjd_v8" }</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -7685,7 +7688,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7764,6 +7767,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -7807,7 +7816,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -8011,6 +8020,12 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -10451,11 +10466,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM476"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="V374" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="1" topLeftCell="V364" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z386" sqref="Z386"/>
+      <selection pane="bottomRight" activeCell="X386" sqref="X386:Y394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.5" x14ac:dyDescent="0.2"/>
@@ -40690,8 +40705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -41336,10 +41351,10 @@
       </c>
     </row>
     <row r="45" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="12">
+      <c r="A45" s="68">
         <v>44</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="69" t="s">
         <v>1762</v>
       </c>
       <c r="C45" s="12">
@@ -41350,10 +41365,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="12">
+      <c r="A46" s="68">
         <v>45</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="69" t="s">
         <v>1763</v>
       </c>
       <c r="C46" s="12">
@@ -41364,10 +41379,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="12">
+      <c r="A47" s="68">
         <v>46</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="69" t="s">
         <v>1764</v>
       </c>
       <c r="C47" s="12">

</xml_diff>